<commit_message>
New code structure is working
</commit_message>
<xml_diff>
--- a/regionalization_experiments.xlsx
+++ b/regionalization_experiments.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
-  <si>
-    <t>Method</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -40,12 +37,6 @@
     <t>idw</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Local_prec_corr</t>
   </si>
   <si>
@@ -53,6 +44,15 @@
   </si>
   <si>
     <t>Run_experiment</t>
+  </si>
+  <si>
+    <t>Reg_method</t>
+  </si>
+  <si>
+    <t>Cmb_method</t>
+  </si>
+  <si>
+    <t>output_average</t>
   </si>
 </sst>
 </file>
@@ -403,161 +403,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
       <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting with spatial_prox and param_average
</commit_message>
<xml_diff>
--- a/regionalization_experiments.xlsx
+++ b/regionalization_experiments.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -506,10 +506,10 @@
         <v>1</v>
       </c>
       <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -529,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
         <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>0</v>

</xml_diff>